<commit_message>
updated priority of backlog
</commit_message>
<xml_diff>
--- a/doc/task10/scrum.xlsx
+++ b/doc/task10/scrum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="120" windowWidth="16485" windowHeight="9315" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="120" windowWidth="16485" windowHeight="9315" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Scrum Master</t>
   </si>
   <si>
-    <t>Das Hauptmenü der App anzeigen, inkl. Daily Events</t>
-  </si>
-  <si>
     <t>Hauptmenü anzeigen</t>
   </si>
   <si>
@@ -183,15 +180,6 @@
     <t>anzeigen Live Up aktivitäen</t>
   </si>
   <si>
-    <t xml:space="preserve">Erinnerung Medikation </t>
-  </si>
-  <si>
-    <t>Auflisten von allen verschriebenen Medikamenten, dosis, einnahme, ect</t>
-  </si>
-  <si>
-    <t>anzeigen der medikation</t>
-  </si>
-  <si>
     <t>Kalender mit Terminübersicht</t>
   </si>
   <si>
@@ -259,6 +247,24 @@
   </si>
   <si>
     <t>MVP Pattern implementieren, mit PatientenApp verknüpfen</t>
+  </si>
+  <si>
+    <t>Das Hauptmenü der App anzeigen, inkl. Daily Events User kann navigieren; user werden daily events angezeigt</t>
+  </si>
+  <si>
+    <t>Auflisten von allen verschriebenen Medikamenten, dosis: user kann medikation ansehen</t>
+  </si>
+  <si>
+    <t>Erinnerung Medikation : Patient wird über medikation erinnert</t>
+  </si>
+  <si>
+    <t>anzeigen der medikation: User wird Medikation angezeit</t>
+  </si>
+  <si>
+    <t>ver high</t>
+  </si>
+  <si>
+    <t>created</t>
   </si>
 </sst>
 </file>
@@ -316,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -331,6 +337,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -635,7 +644,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +667,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -669,57 +678,57 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -729,10 +738,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,10 +787,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -789,56 +798,68 @@
       <c r="E2" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H2" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
+        <v>21</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H3" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>55</v>
+        <v>22</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H4" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
+        <v>23</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>5</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -846,50 +867,59 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
+        <v>24</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>59</v>
+        <v>25</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
+        <v>32</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>15</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -897,50 +927,59 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>61</v>
+        <v>31</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>62</v>
+        <v>26</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>63</v>
+        <v>27</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11">
         <v>10</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -948,16 +987,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
+        <v>28</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
         <v>10</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -965,16 +1007,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>53</v>
+        <v>29</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
         <v>5</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -982,10 +1027,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
+        <v>30</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -993,16 +1038,19 @@
       <c r="E14">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
+        <v>34</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1010,53 +1058,24 @@
       <c r="E15">
         <v>55</v>
       </c>
+      <c r="H15" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A16" s="1">
         <v>17</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="5">
+      <c r="D16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="5">
         <f>180 - SUM(E2:E15)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1068,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,19 +1153,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -1163,19 +1182,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
@@ -1192,19 +1211,19 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
         <v>5</v>
@@ -1221,19 +1240,19 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
         <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" t="s">
-        <v>39</v>
       </c>
       <c r="H5" t="s">
         <v>5</v>
@@ -1250,19 +1269,19 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
         <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>39</v>
       </c>
       <c r="H6" t="s">
         <v>5</v>
@@ -1279,22 +1298,22 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
         <v>38</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>39</v>
       </c>
-      <c r="G7" t="s">
-        <v>40</v>
-      </c>
       <c r="H7" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="I7">
         <v>4</v>
@@ -1308,19 +1327,19 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H8" t="s">
         <v>6</v>
@@ -1332,7 +1351,7 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5">

</xml_diff>

<commit_message>
updated scrumlog, commented interfacnes
</commit_message>
<xml_diff>
--- a/doc/task10/scrum.xlsx
+++ b/doc/task10/scrum.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="120" windowWidth="16485" windowHeight="9315" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="120" windowWidth="16485" windowHeight="9315" tabRatio="662" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
     <sheet name="Product Backlog" sheetId="1" r:id="rId2"/>
-    <sheet name="Sprint Backlog" sheetId="2" r:id="rId3"/>
+    <sheet name="Sprint 1 Backlog" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -258,22 +258,22 @@
     <t>anzeigen der medikation: User wird Medikation angezeit</t>
   </si>
   <si>
-    <t>ver high</t>
-  </si>
-  <si>
     <t>created</t>
   </si>
   <si>
     <t>in progress</t>
   </si>
   <si>
-    <t>review</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
     <t>MVP Pattern emergency  implementieren, mit PatientenApp verknüpfen</t>
+  </si>
+  <si>
+    <t>very high</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -749,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,8 +807,11 @@
       <c r="E2" s="1">
         <v>30</v>
       </c>
+      <c r="G2" s="1">
+        <v>13</v>
+      </c>
       <c r="H2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -828,7 +831,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -848,7 +851,7 @@
         <v>5</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -868,7 +871,7 @@
         <v>5</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -888,7 +891,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -908,7 +911,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -928,7 +931,7 @@
         <v>15</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -948,7 +951,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -968,7 +971,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -988,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1008,7 +1011,7 @@
         <v>10</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1028,7 +1031,7 @@
         <v>5</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1048,7 +1051,7 @@
         <v>15</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1068,7 +1071,7 @@
         <v>55</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1096,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,7 +1112,7 @@
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" customWidth="1"/>
     <col min="11" max="11" width="7.28515625" customWidth="1"/>
@@ -1189,7 +1192,7 @@
         <v>7</v>
       </c>
       <c r="L2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1203,7 +1206,7 @@
         <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
         <v>37</v>
@@ -1220,8 +1223,11 @@
       <c r="I3">
         <v>4</v>
       </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
       <c r="L3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
@@ -1253,7 +1259,7 @@
         <v>6</v>
       </c>
       <c r="L4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1284,8 +1290,14 @@
       <c r="I5">
         <v>2</v>
       </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
       <c r="L5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1316,8 +1328,14 @@
       <c r="I6">
         <v>4</v>
       </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
       <c r="L6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1343,13 +1361,13 @@
         <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I7">
         <v>4</v>
       </c>
       <c r="L7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1379,6 +1397,9 @@
       </c>
       <c r="I8">
         <v>4</v>
+      </c>
+      <c r="K8" t="s">
+        <v>85</v>
       </c>
       <c r="L8" t="s">
         <v>82</v>
@@ -1396,11 +1417,11 @@
       </c>
       <c r="J10">
         <f>SUM(J2:J9)</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="K10">
         <f>SUM(K2:K9)</f>
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>